<commit_message>
MOSIP-29415 Added location for spa language.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_hierarchy_list.xlsx
+++ b/mosip_master/xlsx/loc_hierarchy_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17190E33-073C-4773-B1C5-40B8570035F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DA9B8F-05DD-4527-BF46-F1C33504D9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
     <t>Zona</t>
   </si>
   <si>
-    <t>Código Postal</t>
+    <t xml:space="preserve"> Código Postal</t>
   </si>
 </sst>
 </file>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,7 +1175,7 @@
       <c r="B43">
         <v>5</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" t="s">
         <v>51</v>
       </c>
       <c r="D43" s="1" t="s">

</xml_diff>

<commit_message>
MOSIP-29415 Fixed Foreign key constraint issue for Location code cardigo portal in spanish language.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_hierarchy_list.xlsx
+++ b/mosip_master/xlsx/loc_hierarchy_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17190E33-073C-4773-B1C5-40B8570035F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987E270E-8711-441F-A8F3-D7BA84F14BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
     <t>Zona</t>
   </si>
   <si>
-    <t>Código Postal</t>
+    <t xml:space="preserve"> Código Postal</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,7 +1175,7 @@
       <c r="B43">
         <v>5</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" t="s">
         <v>51</v>
       </c>
       <c r="D43" s="1" t="s">

</xml_diff>